<commit_message>
Se agrego un archivo resumen con todas las librerias utilizadas
</commit_message>
<xml_diff>
--- a/niveles_cuantizacion.xlsx
+++ b/niveles_cuantizacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMACION\Practicas\python\converter-ad-da\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252785EF-70DD-42A1-965A-EF1D7066E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C099CA2C-EE3E-4E27-900D-5DC4097586EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{65B5CFF8-0150-40D7-B22E-7EDFD37D5C72}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13935" windowHeight="16200" xr2:uid="{65B5CFF8-0150-40D7-B22E-7EDFD37D5C72}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuantización" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -131,10 +131,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -454,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DFAC55-67D6-436D-B24F-56A251280095}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +609,7 @@
       <c r="A17" s="3">
         <v>0</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" s="1"/>
@@ -633,155 +629,189 @@
       <c r="Q17" s="1"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>-1</v>
       </c>
-      <c r="B18" s="7">
-        <f>B17-$B$35</f>
+      <c r="B18" s="5">
+        <f>B17-$F$31</f>
         <v>-0.75</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>-2</v>
       </c>
-      <c r="B19" s="8">
-        <f t="shared" ref="B19:B33" si="1">B18-$B$35</f>
+      <c r="B19" s="6">
+        <f>B18-$F$31</f>
         <v>-1.5</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>-3</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
+        <f>B19-$F$31</f>
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>-4</v>
+      </c>
+      <c r="B21" s="6">
+        <f>B20-$F$31</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>-5</v>
+      </c>
+      <c r="B22" s="6">
+        <f>B21-$F$31</f>
+        <v>-3.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>-6</v>
+      </c>
+      <c r="B23" s="6">
+        <f>B22-$F$31</f>
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>-7</v>
+      </c>
+      <c r="B24" s="6">
+        <f>B23-$F$31</f>
+        <v>-5.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>-8</v>
+      </c>
+      <c r="B25" s="6">
+        <f>B24-$F$31</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>-9</v>
+      </c>
+      <c r="B26" s="6">
+        <f>B25-$F$31</f>
+        <v>-6.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>-10</v>
+      </c>
+      <c r="B27" s="6">
+        <f>B26-$F$31</f>
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>-11</v>
+      </c>
+      <c r="B28" s="6">
+        <f>B27-$F$31</f>
+        <v>-8.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>-12</v>
+      </c>
+      <c r="B29" s="6">
+        <f>B28-$F$31</f>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>-13</v>
+      </c>
+      <c r="B30" s="6">
+        <f>B29-$F$31</f>
+        <v>-9.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>-14</v>
+      </c>
+      <c r="B31" s="6">
+        <f>B30-$F$31</f>
+        <v>-10.5</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>-15</v>
+      </c>
+      <c r="B32" s="6">
+        <f>B31-$F$31</f>
+        <v>-11.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>-16</v>
+      </c>
+      <c r="B33" s="6">
+        <f>B32-$F$31</f>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <f t="shared" ref="B34:B39" si="1">B33-$F$31</f>
+        <v>-12.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
         <f t="shared" si="1"/>
-        <v>-2.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>-4</v>
-      </c>
-      <c r="B21" s="8">
+        <v>-13.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
         <f t="shared" si="1"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>-5</v>
-      </c>
-      <c r="B22" s="8">
+        <v>-14.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
         <f t="shared" si="1"/>
-        <v>-3.75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>-6</v>
-      </c>
-      <c r="B23" s="8">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
         <f t="shared" si="1"/>
-        <v>-4.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>-7</v>
-      </c>
-      <c r="B24" s="8">
+        <v>-15.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
         <f t="shared" si="1"/>
-        <v>-5.25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>-8</v>
-      </c>
-      <c r="B25" s="8">
-        <f t="shared" si="1"/>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>-9</v>
-      </c>
-      <c r="B26" s="8">
-        <f t="shared" si="1"/>
-        <v>-6.75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>-10</v>
-      </c>
-      <c r="B27" s="8">
-        <f t="shared" si="1"/>
-        <v>-7.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>-11</v>
-      </c>
-      <c r="B28" s="8">
-        <f t="shared" si="1"/>
-        <v>-8.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>-12</v>
-      </c>
-      <c r="B29" s="8">
-        <f t="shared" si="1"/>
-        <v>-9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>-13</v>
-      </c>
-      <c r="B30" s="8">
-        <f t="shared" si="1"/>
-        <v>-9.75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>-14</v>
-      </c>
-      <c r="B31" s="8">
-        <f t="shared" si="1"/>
-        <v>-10.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>-15</v>
-      </c>
-      <c r="B32" s="8">
-        <f t="shared" si="1"/>
-        <v>-11.25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>-16</v>
-      </c>
-      <c r="B33" s="8">
-        <f t="shared" si="1"/>
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>0.75</v>
+        <v>-16.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>